<commit_message>
excel graphs formatting for report
</commit_message>
<xml_diff>
--- a/bo_mf_opt_results.xlsx
+++ b/bo_mf_opt_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoetan/Documents/Cambridge/IIB/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A860EBC1-28E8-6A46-89A6-3E24E6E84F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FFFA43-549C-F54D-9C39-F0E4478173AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19840" xr2:uid="{13FA511A-9E78-4540-AAF4-BA27591AA27A}"/>
   </bookViews>
@@ -152,6 +152,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDADADA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -8748,9 +8753,7 @@
     </a:solidFill>
     <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:tint val="75000"/>
-        </a:schemeClr>
+        <a:srgbClr val="DADADA"/>
       </a:solidFill>
       <a:prstDash val="solid"/>
       <a:round/>
@@ -9266,16 +9269,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>114306</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>269</xdr:row>
+      <xdr:rowOff>152406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
-      <xdr:row>303</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14686,7 +14689,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A264" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T278" sqref="T278"/>
+      <selection pane="bottomLeft" activeCell="X282" sqref="X282:X283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>